<commit_message>
Merapikan file & memindahkan sempro dan semhas ke folder masing - masing
</commit_message>
<xml_diff>
--- a/Dokumen Pelengkap/Akurasi.xlsx
+++ b/Dokumen Pelengkap/Akurasi.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,53 +37,53 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
   <si>
+    <t>SVM Kernel Linear</t>
+  </si>
+  <si>
+    <t>SVM Kernel RBF</t>
+  </si>
+  <si>
+    <t>Klasifikasi</t>
+  </si>
+  <si>
+    <t>Akurasi</t>
+  </si>
+  <si>
     <t>Kelas</t>
   </si>
   <si>
+    <t>Prediksi</t>
+  </si>
+  <si>
+    <t>0.921995 (92.2%)</t>
+  </si>
+  <si>
+    <t>Negatif</t>
+  </si>
+  <si>
+    <t>Positif</t>
+  </si>
+  <si>
+    <t>0.917519 (91.8%)</t>
+  </si>
+  <si>
     <t>Aktual</t>
   </si>
   <si>
-    <t>Prediksi</t>
-  </si>
-  <si>
-    <t>Positif</t>
-  </si>
-  <si>
-    <t>Negatif</t>
-  </si>
-  <si>
-    <t>SVM Kernel Linear</t>
-  </si>
-  <si>
-    <t>SVM Kernel RBF</t>
+    <t>KNN dengan K = 4</t>
+  </si>
+  <si>
+    <t>0.753197 (75.3%)</t>
   </si>
   <si>
     <t>KNN K = 5</t>
-  </si>
-  <si>
-    <t>Klasifikasi</t>
-  </si>
-  <si>
-    <t>Akurasi</t>
-  </si>
-  <si>
-    <t>KNN dengan K = 4</t>
-  </si>
-  <si>
-    <t>0.921995 (92.2%)</t>
-  </si>
-  <si>
-    <t>0.917519 (91.8%)</t>
-  </si>
-  <si>
-    <t>0.753197 (75.3%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,23 +135,23 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,7 +472,7 @@
       <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="2" max="2" width="5" customWidth="1"/>
@@ -480,185 +481,189 @@
     <col min="13" max="13" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="2:13">
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="G1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="L1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" ht="15" customHeight="1">
+      <c r="B2" s="5"/>
+      <c r="C2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="E2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="L2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="L1" s="6" t="s">
+    </row>
+    <row r="3" spans="2:13" ht="15" customHeight="1">
+      <c r="B3" s="5"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="G3" s="5"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="2"/>
-      <c r="L2" s="7" t="s">
+    <row r="4" spans="2:13" ht="20.100000000000001" customHeight="1">
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1256</v>
+      </c>
+      <c r="E4" s="1">
+        <v>26</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1272</v>
+      </c>
+      <c r="J4" s="1">
+        <v>10</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="20.100000000000001" customHeight="1">
+      <c r="B5" s="4"/>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1">
+        <v>96</v>
+      </c>
+      <c r="E5" s="1">
+        <v>186</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="1">
+        <v>119</v>
+      </c>
+      <c r="J5" s="1">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="15" customHeight="1"/>
+    <row r="7" spans="2:13">
+      <c r="B7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="B8" s="5"/>
+      <c r="C8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1256</v>
-      </c>
-      <c r="E4" s="4">
-        <v>26</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="4">
-        <v>1272</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="2:13">
+      <c r="B9" s="5"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="20.100000000000001" customHeight="1">
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-      <c r="C5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="4">
-        <v>96</v>
-      </c>
-      <c r="E5" s="4">
-        <v>186</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="4">
-        <v>119</v>
-      </c>
-      <c r="J5" s="4">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="D10" s="1">
         <v>932</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="1">
         <v>350</v>
       </c>
     </row>
-    <row r="11" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="4">
+    <row r="11" spans="2:13" ht="20.100000000000001" customHeight="1">
+      <c r="B11" s="4"/>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1">
         <v>36</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="1">
         <v>246</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:J2"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B2:B3"/>
@@ -670,10 +675,6 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Mengupdate File Skripsi ke Versi Final & Mengubah Beberapa File - Menambahkan file Skripsi dan Paper serta File Pendukungnya - Mengubah file Akurasi.xlsx dikarenakan perubahan hasil - Menghapus file Referensi untuk mencegah terkena copyright
</commit_message>
<xml_diff>
--- a/Dokumen Pelengkap/Akurasi.xlsx
+++ b/Dokumen Pelengkap/Akurasi.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/39f26c447bd92883/Dokumen/Tugas Kuliah/Skripsi/Dokumen Pelengkap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89BBF3B2-DCD7-4BFA-A025-6B55EE303FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{89BBF3B2-DCD7-4BFA-A025-6B55EE303FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{840EA910-7253-418C-B91F-1F45EB0BA56F}"/>
   <bookViews>
     <workbookView xWindow="2895" yWindow="3765" windowWidth="21600" windowHeight="11385" xr2:uid="{4D6CAEDD-C134-47CB-936E-C5917036289E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Akurasi" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -55,7 +55,7 @@
     <t>Prediksi</t>
   </si>
   <si>
-    <t>0.921995 (92.2%)</t>
+    <t>0.938619 (93.9%)</t>
   </si>
   <si>
     <t>Negatif</t>
@@ -64,7 +64,7 @@
     <t>Positif</t>
   </si>
   <si>
-    <t>0.917519 (91.8%)</t>
+    <t>0.927109 (92.7%)</t>
   </si>
   <si>
     <t>Aktual</t>
@@ -73,10 +73,10 @@
     <t>KNN dengan K = 4</t>
   </si>
   <si>
-    <t>0.753197 (75.3%)</t>
-  </si>
-  <si>
-    <t>KNN K = 5</t>
+    <t>0.888107 (88.8%)</t>
+  </si>
+  <si>
+    <t>KNN K = 4</t>
   </si>
 </sst>
 </file>
@@ -140,17 +140,17 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,7 +469,7 @@
   <dimension ref="B1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -482,18 +482,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="G1" s="6" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="G1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
       <c r="L1" s="2" t="s">
         <v>2</v>
       </c>
@@ -502,22 +502,22 @@
       </c>
     </row>
     <row r="2" spans="2:13" ht="15" customHeight="1">
-      <c r="B2" s="5"/>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="7" t="s">
+      <c r="E2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="5"/>
+      <c r="J2" s="6"/>
       <c r="L2" s="3" t="s">
         <v>0</v>
       </c>
@@ -526,16 +526,16 @@
       </c>
     </row>
     <row r="3" spans="2:13" ht="15" customHeight="1">
-      <c r="B3" s="5"/>
-      <c r="C3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="5"/>
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="7"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="5"/>
       <c r="I3" s="1" t="s">
         <v>7</v>
       </c>
@@ -550,29 +550,29 @@
       </c>
     </row>
     <row r="4" spans="2:13" ht="20.100000000000001" customHeight="1">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="1">
-        <v>1256</v>
+        <v>260</v>
       </c>
       <c r="E4" s="1">
-        <v>26</v>
-      </c>
-      <c r="G4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="1">
-        <v>1272</v>
+        <v>242</v>
       </c>
       <c r="J4" s="1">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>11</v>
@@ -582,49 +582,49 @@
       </c>
     </row>
     <row r="5" spans="2:13" ht="20.100000000000001" customHeight="1">
-      <c r="B5" s="4"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="1">
-        <v>96</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1">
-        <v>186</v>
-      </c>
-      <c r="G5" s="4"/>
+        <v>1208</v>
+      </c>
+      <c r="G5" s="7"/>
       <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="1">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="J5" s="1">
-        <v>163</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="15" customHeight="1"/>
     <row r="7" spans="2:13">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="2:13">
-      <c r="B8" s="5"/>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="2:13">
-      <c r="B9" s="5"/>
-      <c r="C9" s="7"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
@@ -633,29 +633,29 @@
       </c>
     </row>
     <row r="10" spans="2:13" ht="20.100000000000001" customHeight="1">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="1">
-        <v>932</v>
+        <v>143</v>
       </c>
       <c r="E10" s="1">
-        <v>350</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="20.100000000000001" customHeight="1">
-      <c r="B11" s="4"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="1">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E11" s="1">
-        <v>246</v>
+        <v>1246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>